<commit_message>
ACCUSTOM JSAC 2024: Preparing scripts for the JSAC extensions; Minor bug fixes in UAV mobility power model
</commit_message>
<xml_diff>
--- a/test/custom/reward_model_power.xlsx
+++ b/test/custom/reward_model_power.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\Hermes\test\custom\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE4A8E4-1D8D-4880-8B53-6608863395D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Plotly" sheetId="1" r:id="rId1"/>
-    <sheet name="ACCUSTOM_1_Grid" sheetId="2" r:id="rId2"/>
+    <sheet name="reward_model_power" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>https://plotly.com/~total.academe/179/</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>A</t>
   </si>
@@ -42,44 +44,19 @@
   </si>
   <si>
     <t>H</t>
-  </si>
-  <si>
-    <t>1,319.59</t>
-  </si>
-  <si>
-    <t>1,086.31</t>
-  </si>
-  <si>
-    <t>1,119.87</t>
-  </si>
-  <si>
-    <t>1,277.69</t>
-  </si>
-  <si>
-    <t>1,333.94</t>
-  </si>
-  <si>
-    <t>1,467.49</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -116,76 +93,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="381000"/>
-          <a:ext cx="6667500" cy="4762500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -223,7 +162,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -257,6 +196,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -291,9 +231,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -466,208 +407,268 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="34.36328125" customWidth="1"/>
+    <col min="2" max="2" width="34.54296875" customWidth="1"/>
+    <col min="3" max="3" width="38.90625" customWidth="1"/>
+    <col min="4" max="4" width="31.1796875" customWidth="1"/>
+    <col min="5" max="5" width="46.81640625" customWidth="1"/>
+    <col min="6" max="6" width="39.453125" customWidth="1"/>
+    <col min="7" max="7" width="39.54296875" customWidth="1"/>
+    <col min="8" max="8" width="36" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
         <v>1000</v>
       </c>
-      <c r="E2">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2">
         <v>752.55</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>2000</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
         <v>1100</v>
       </c>
-      <c r="E3">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2">
         <v>842.47</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>2375</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4">
-        <v>1107.66</v>
-      </c>
-      <c r="D4">
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>1107.6600000000001</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2">
         <v>488.01</v>
       </c>
-      <c r="F4">
+      <c r="E4" s="2"/>
+      <c r="F4" s="2">
         <v>2411.66</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5">
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
         <v>1200</v>
       </c>
-      <c r="E5">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
         <v>924.52</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>2750</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="F6">
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2">
         <v>3031.44</v>
       </c>
-      <c r="H6">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2">
         <v>732.09</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
         <v>1300</v>
       </c>
-      <c r="E7">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
         <v>976.02</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>3125</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="F8">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2">
         <v>3200</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>689.62</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>1319.59</v>
+      </c>
+      <c r="B9" s="2">
         <v>600.63</v>
       </c>
-      <c r="F9">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2">
         <v>3219.59</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10">
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
         <v>1371.32</v>
       </c>
-      <c r="C10">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2">
         <v>561.21</v>
       </c>
-      <c r="F10">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2">
         <v>3371.32</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11">
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
         <v>1400</v>
       </c>
-      <c r="E11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2">
+        <v>1086.31</v>
+      </c>
+      <c r="F11" s="2">
         <v>3500</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12">
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
         <v>1500</v>
       </c>
-      <c r="E12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2">
+        <v>1119.8699999999999</v>
+      </c>
+      <c r="F12" s="2">
         <v>3875</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13">
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
         <v>1600</v>
       </c>
-      <c r="E13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2">
+        <v>1277.69</v>
+      </c>
+      <c r="F13" s="2">
         <v>4250</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14">
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
         <v>1700</v>
       </c>
-      <c r="E14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2">
+        <v>1333.94</v>
+      </c>
+      <c r="F14" s="2">
         <v>4625</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15">
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
         <v>1800</v>
       </c>
-      <c r="E15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2">
+        <v>1467.49</v>
+      </c>
+      <c r="F15" s="2">
         <v>5000</v>
       </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>